<commit_message>
carga masiva insertar y actualizar productos
</commit_message>
<xml_diff>
--- a/eCommerce.Web/Content/bm3/excel-format/Products.xlsx
+++ b/eCommerce.Web/Content/bm3/excel-format/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SISTEMAS\eCommerceMotos\Leder\EcommerceMotos\eCommerce.Web\Content\bm3\excel-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCE1AD2-7D3A-4834-9663-8AFE6BC2C25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6202AD-EB69-4375-9937-0CA7DC86A9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E60018BB-DC7F-43F8-AE4F-26BFB686967E}"/>
   </bookViews>
@@ -25,50 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Descuento</t>
-  </si>
-  <si>
-    <t>Costo</t>
-  </si>
-  <si>
-    <t>SKU</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Proveedor</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>IsActive</t>
-  </si>
-  <si>
-    <t>IsDeleted</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>EtiquetaOferta</t>
-  </si>
-  <si>
-    <t>IDCatalogo</t>
-  </si>
-  <si>
-    <t>TipoMoneda</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,59 +375,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5273473C-D952-4204-A8C5-20B7FA9B2176}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>